<commit_message>
plots generated for the paper
</commit_message>
<xml_diff>
--- a/data/sets/Round2/PPSet5.xlsx
+++ b/data/sets/Round2/PPSet5.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\OneDrive\Desktop\LASIR\USB Microscope Picture\S5_parts\PPSet5\Round2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kapusub\git\Bayesian-Neural-Network\data\sets\Round2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{0322B2A2-77B9-4C6B-932F-BBE3DEFBF12C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7C77DF9-C540-486F-8C12-9579287A4CEB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC445E8D-E238-4F7F-A0A4-D41A9847C0EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9990" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="B" sheetId="1" r:id="rId1"/>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,7 +74,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +84,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -101,11 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,11 +425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11760DF-4C23-4EA2-A562-BB0A6E2B36FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="J15" sqref="I15:J28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +816,7 @@
       <c r="C24">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="4">
         <f t="shared" si="0"/>
         <v>7.6199999999999992E-3</v>
       </c>
@@ -1037,7 +1043,7 @@
       <c r="C38" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="4">
         <f t="shared" si="0"/>
         <v>5.0800000000000003E-3</v>
       </c>
@@ -1264,7 +1270,7 @@
       <c r="C52" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="4">
         <f t="shared" si="0"/>
         <v>5.0800000000000003E-3</v>
       </c>
@@ -1475,7 +1481,7 @@
       <c r="C65" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="4">
         <f t="shared" si="0"/>
         <v>1.0160000000000001E-2</v>
       </c>

</xml_diff>